<commit_message>
anova tests added and results are in analysis_result2.xls
</commit_message>
<xml_diff>
--- a/analysis_result2.xlsx
+++ b/analysis_result2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="47">
   <si>
     <t>control_all</t>
   </si>
@@ -116,13 +116,52 @@
   </si>
   <si>
     <t>F 0.02,0.2,0.1</t>
+  </si>
+  <si>
+    <t>F(even) means other than even channels, all tests came out false</t>
+  </si>
+  <si>
+    <t>Even channels start from channel0</t>
+  </si>
+  <si>
+    <t>F(Even,8910)</t>
+  </si>
+  <si>
+    <t>F(8910)</t>
+  </si>
+  <si>
+    <t>F(even,8910,1112)</t>
+  </si>
+  <si>
+    <t>F(even,567,8910,1112)</t>
+  </si>
+  <si>
+    <t>F(Even,8910,1112)</t>
+  </si>
+  <si>
+    <t>F(even,8910)</t>
+  </si>
+  <si>
+    <t>F(11,567)</t>
+  </si>
+  <si>
+    <t>F(13,15,567)</t>
+  </si>
+  <si>
+    <t>F(567)</t>
+  </si>
+  <si>
+    <t>Conclusions:</t>
+  </si>
+  <si>
+    <t>1. Even channels can tell dictinction between athelets and pros, in both two tailed t mean test and anova tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,13 +169,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,13 +199,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,22 +511,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA36"/>
+  <dimension ref="A1:AA41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1141,57 +1198,57 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>4</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>6.4346899999999998</v>
+      <c r="I11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1200,59 +1257,95 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H12">
-        <v>6.1369499999999997</v>
+        <v>5.5998799999999997</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13">
-        <v>6.3647600000000004</v>
+        <v>5.5849500000000001</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1264,21 +1357,39 @@
         <v>7</v>
       </c>
       <c r="H14">
-        <v>3.3973599999999999</v>
+        <v>5.2313099999999997</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -1290,553 +1401,1008 @@
         <v>7</v>
       </c>
       <c r="H15">
-        <v>6.53104</v>
+        <v>5.577</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>5.9243600000000001</v>
+      </c>
+      <c r="I16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16">
-        <v>5.8127599999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>5.7498899999999997</v>
+      </c>
+      <c r="I17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>31</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18">
         <v>6.1947799999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18">
-        <v>6.3548099999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>5.8360200000000004</v>
+      </c>
+      <c r="I19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19">
-        <v>6.7201899999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>6.2050900000000002</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>33</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20">
-        <v>6.4213399999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>6.8341000000000003</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>1234</v>
       </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
         <v>14</v>
       </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21">
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22">
         <v>6.6223400000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>1534</v>
       </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22">
-        <v>4.8806399999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>4.3817899999999996</v>
+      </c>
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>1235</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
         <v>15</v>
       </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23">
-        <v>6.2577100000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>4.88375</v>
+      </c>
+      <c r="I24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K24" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" t="s">
+        <v>6</v>
+      </c>
+      <c r="M24" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>1245</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>17</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>13</v>
       </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24">
-        <v>6.3953699999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>6.7507200000000003</v>
+      </c>
+      <c r="I25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L25" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>1324</v>
       </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25">
-        <v>5.3339699999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>4.7720700000000003</v>
+      </c>
+      <c r="I26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>1325</v>
       </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
         <v>18</v>
       </c>
-      <c r="H26">
-        <v>6.5051500000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="H27">
+        <v>5.1711900000000002</v>
+      </c>
+      <c r="I27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" t="s">
+        <v>43</v>
+      </c>
+      <c r="K27" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>1345</v>
       </c>
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
         <v>19</v>
       </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27">
-        <v>6.4495399999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28">
+        <v>4.7031499999999999</v>
+      </c>
+      <c r="I28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" t="s">
+        <v>6</v>
+      </c>
+      <c r="M28" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>1423</v>
       </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28">
-        <v>6.7118200000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>6.2297700000000003</v>
+      </c>
+      <c r="I29" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" t="s">
+        <v>6</v>
+      </c>
+      <c r="L29" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" t="s">
+        <v>7</v>
+      </c>
+      <c r="N29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>1425</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>21</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>13</v>
       </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29">
-        <v>7.0865549999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>5.79148</v>
+      </c>
+      <c r="I30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" t="s">
+        <v>6</v>
+      </c>
+      <c r="N30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>1435</v>
       </c>
-      <c r="B30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30">
-        <v>6.2869400000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31">
+        <v>5.4109800000000003</v>
+      </c>
+      <c r="I31" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" t="s">
+        <v>6</v>
+      </c>
+      <c r="K31" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>1523</v>
       </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" t="s">
-        <v>6</v>
-      </c>
-      <c r="G31" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31">
-        <v>4.5663600000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32">
+        <v>4.3749900000000004</v>
+      </c>
+      <c r="I32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" t="s">
+        <v>7</v>
+      </c>
+      <c r="N32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>1524</v>
       </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33">
         <v>4.8902599999999996</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="I33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L33" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>1534</v>
       </c>
-      <c r="B33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33">
-        <v>4.8806399999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34">
+        <v>4.3817899999999996</v>
+      </c>
+      <c r="I34" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" t="s">
+        <v>6</v>
+      </c>
+      <c r="K34" t="s">
+        <v>6</v>
+      </c>
+      <c r="L34" t="s">
+        <v>6</v>
+      </c>
+      <c r="M34" t="s">
+        <v>6</v>
+      </c>
+      <c r="N34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>2345</v>
       </c>
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
         <v>13</v>
       </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34">
-        <v>6.9335100000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35">
+        <v>6.7920999999999996</v>
+      </c>
+      <c r="I35" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" t="s">
+        <v>44</v>
+      </c>
+      <c r="L35" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" t="s">
+        <v>7</v>
+      </c>
+      <c r="N35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>2435</v>
       </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" t="s">
-        <v>6</v>
-      </c>
-      <c r="G35" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35">
-        <v>4.9343199999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36">
+        <v>5.4920499999999999</v>
+      </c>
+      <c r="I36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L36" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>2534</v>
       </c>
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
         <v>22</v>
       </c>
-      <c r="E36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36">
-        <v>6.9745400000000002</v>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37">
+        <v>6.5422500000000001</v>
+      </c>
+      <c r="I37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" t="s">
+        <v>6</v>
+      </c>
+      <c r="K37" t="s">
+        <v>6</v>
+      </c>
+      <c r="L37" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" t="s">
+        <v>7</v>
+      </c>
+      <c r="N37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>